<commit_message>
added english template, deployed calculator
</commit_message>
<xml_diff>
--- a/static/template_en.xlsx
+++ b/static/template_en.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tducrot/tdr2d/ovh_pricelist/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF57D7F-806F-E14B-B82C-E3B43B09E275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7F2AA5-3BA9-0242-848D-66C34F8C5992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12214,6 +12214,61 @@
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="36" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="28" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" xfId="47" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="18" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="20" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="24" borderId="15" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="24" borderId="16" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="24" borderId="20" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="24" borderId="19" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -12265,61 +12320,6 @@
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="18" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="20" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="15" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="16" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="20" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="19" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="28" borderId="0" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" xfId="47" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="62">
     <cellStyle name="%" xfId="48" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -12753,8 +12753,8 @@
   </sheetPr>
   <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -13352,18 +13352,18 @@
       <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="20">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="110"/>
+      <c r="B2" s="128"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="128"/>
+      <c r="F2" s="128"/>
+      <c r="G2" s="128"/>
+      <c r="H2" s="128"/>
+      <c r="I2" s="128"/>
+      <c r="J2" s="129"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="66"/>
@@ -13385,13 +13385,13 @@
         <v>14</v>
       </c>
       <c r="F5" s="100"/>
-      <c r="G5" s="111">
+      <c r="G5" s="130">
         <f ca="1">NOW()</f>
-        <v>45182.557190624997</v>
+        <v>45182.577693055558</v>
       </c>
-      <c r="H5" s="111"/>
-      <c r="I5" s="111"/>
-      <c r="J5" s="112"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="131"/>
     </row>
     <row r="6" spans="1:10" ht="55" customHeight="1">
       <c r="B6" s="105" t="s">
@@ -13416,10 +13416,10 @@
         <v>16</v>
       </c>
       <c r="F7" s="104"/>
-      <c r="G7" s="113"/>
-      <c r="H7" s="113"/>
-      <c r="I7" s="113"/>
-      <c r="J7" s="114"/>
+      <c r="G7" s="132"/>
+      <c r="H7" s="132"/>
+      <c r="I7" s="132"/>
+      <c r="J7" s="133"/>
     </row>
     <row r="8" spans="1:10" ht="14">
       <c r="C8" s="68">
@@ -13427,22 +13427,22 @@
       </c>
     </row>
     <row r="9" spans="1:10" s="6" customFormat="1" ht="14">
-      <c r="A9" s="115" t="s">
+      <c r="A9" s="134" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="116"/>
+      <c r="B9" s="135"/>
       <c r="C9" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="115" t="s">
+      <c r="D9" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="117"/>
-      <c r="F9" s="117"/>
-      <c r="G9" s="117"/>
-      <c r="H9" s="117"/>
-      <c r="I9" s="117"/>
-      <c r="J9" s="116"/>
+      <c r="E9" s="136"/>
+      <c r="F9" s="136"/>
+      <c r="G9" s="136"/>
+      <c r="H9" s="136"/>
+      <c r="I9" s="136"/>
+      <c r="J9" s="135"/>
     </row>
     <row r="10" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
       <c r="A10" s="61" t="s">
@@ -13452,15 +13452,15 @@
       <c r="C10" s="89">
         <v>10</v>
       </c>
-      <c r="D10" s="118" t="s">
+      <c r="D10" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="119"/>
-      <c r="F10" s="119"/>
-      <c r="G10" s="119"/>
-      <c r="H10" s="119"/>
-      <c r="I10" s="119"/>
-      <c r="J10" s="120"/>
+      <c r="E10" s="138"/>
+      <c r="F10" s="138"/>
+      <c r="G10" s="138"/>
+      <c r="H10" s="138"/>
+      <c r="I10" s="138"/>
+      <c r="J10" s="139"/>
     </row>
     <row r="11" spans="1:10" s="6" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="37" t="s">
@@ -13470,10 +13470,10 @@
       <c r="C11" s="89">
         <v>250</v>
       </c>
-      <c r="D11" s="121"/>
-      <c r="E11" s="122"/>
-      <c r="F11" s="122"/>
-      <c r="G11" s="122"/>
+      <c r="D11" s="140"/>
+      <c r="E11" s="141"/>
+      <c r="F11" s="141"/>
+      <c r="G11" s="141"/>
       <c r="H11" s="39"/>
       <c r="J11" s="8"/>
     </row>
@@ -13483,11 +13483,11 @@
       </c>
       <c r="B12" s="41"/>
       <c r="C12" s="89">
-        <v>1</v>
+        <v>0</v>
       </c>
-      <c r="D12" s="106"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
+      <c r="D12" s="125"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
       <c r="G12" s="36"/>
       <c r="H12" s="36"/>
       <c r="I12" s="36"/>
@@ -13501,21 +13501,21 @@
       <c r="C13" s="89">
         <v>12</v>
       </c>
-      <c r="D13" s="127"/>
-      <c r="E13" s="128"/>
-      <c r="F13" s="128"/>
-      <c r="G13" s="128"/>
-      <c r="H13" s="128"/>
-      <c r="I13" s="128"/>
-      <c r="J13" s="129"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="114"/>
+      <c r="F13" s="114"/>
+      <c r="G13" s="114"/>
+      <c r="H13" s="114"/>
+      <c r="I13" s="114"/>
+      <c r="J13" s="115"/>
     </row>
     <row r="15" spans="1:10" s="6" customFormat="1" ht="73.5" customHeight="1">
-      <c r="A15" s="134" t="s">
+      <c r="A15" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="135"/>
-      <c r="C15" s="135"/>
-      <c r="D15" s="136"/>
+      <c r="B15" s="121"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="122"/>
       <c r="E15" s="50" t="s">
         <v>20</v>
       </c>
@@ -13538,26 +13538,26 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1">
-      <c r="A16" s="130" t="s">
+      <c r="A16" s="116" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="131"/>
-      <c r="C16" s="131"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="132"/>
-      <c r="F16" s="132"/>
-      <c r="G16" s="132"/>
-      <c r="H16" s="132"/>
-      <c r="I16" s="132"/>
-      <c r="J16" s="133"/>
+      <c r="B16" s="117"/>
+      <c r="C16" s="117"/>
+      <c r="D16" s="117"/>
+      <c r="E16" s="118"/>
+      <c r="F16" s="118"/>
+      <c r="G16" s="118"/>
+      <c r="H16" s="118"/>
+      <c r="I16" s="118"/>
+      <c r="J16" s="119"/>
     </row>
     <row r="17" spans="1:10" ht="122" customHeight="1">
-      <c r="A17" s="137" t="s">
+      <c r="A17" s="123" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="138"/>
-      <c r="C17" s="138"/>
-      <c r="D17" s="138"/>
+      <c r="B17" s="124"/>
+      <c r="C17" s="124"/>
+      <c r="D17" s="124"/>
       <c r="E17" s="33">
         <v>10</v>
       </c>
@@ -13638,7 +13638,7 @@
       <c r="C22" s="6"/>
       <c r="D22" s="84" t="str">
         <f>IF(C12&gt;0,"Exceptional Discount (-"&amp;C12&amp;"%)","")</f>
-        <v>Exceptional Discount (-1%)</v>
+        <v/>
       </c>
       <c r="E22" s="86"/>
       <c r="F22" s="86"/>
@@ -13647,7 +13647,7 @@
       <c r="I22" s="86"/>
       <c r="J22" s="60">
         <f>(0-J20-J21)*($C$12/100)</f>
-        <v>-29.06915</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="16" customHeight="1">
@@ -13665,7 +13665,7 @@
       <c r="I23" s="86"/>
       <c r="J23" s="59">
         <f>J20+J21+J22</f>
-        <v>2877.8458500000002</v>
+        <v>2906.915</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="14" customHeight="1">
@@ -13698,7 +13698,7 @@
       <c r="I25" s="86"/>
       <c r="J25" s="57">
         <f>J23*(1+$C$8/100)</f>
-        <v>3453.4150199999999</v>
+        <v>3488.2979999999998</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
@@ -13730,7 +13730,7 @@
       <c r="I27" s="86"/>
       <c r="J27" s="45">
         <f>J23*$C$13+J24</f>
-        <v>34544.150200000004</v>
+        <v>34892.979999999996</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="6" customFormat="1" ht="15.5" customHeight="1">
@@ -13746,7 +13746,7 @@
       <c r="I28" s="88"/>
       <c r="J28" s="58">
         <f>J27*1.2</f>
-        <v>41452.980240000004</v>
+        <v>41871.575999999994</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="14">
@@ -13780,8 +13780,8 @@
       <c r="J31" s="29"/>
     </row>
     <row r="32" spans="1:10" ht="14">
-      <c r="A32" s="125"/>
-      <c r="B32" s="126"/>
+      <c r="A32" s="111"/>
+      <c r="B32" s="112"/>
       <c r="C32" s="30"/>
       <c r="D32" s="30"/>
       <c r="E32" s="30"/>
@@ -13848,10 +13848,10 @@
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
-      <c r="G37" s="123"/>
-      <c r="H37" s="123"/>
-      <c r="I37" s="123"/>
-      <c r="J37" s="124"/>
+      <c r="G37" s="109"/>
+      <c r="H37" s="109"/>
+      <c r="I37" s="109"/>
+      <c r="J37" s="110"/>
     </row>
     <row r="38" spans="1:10" ht="14">
       <c r="A38" s="37"/>
@@ -13859,10 +13859,10 @@
       <c r="C38" s="7"/>
       <c r="D38" s="5"/>
       <c r="F38" s="6"/>
-      <c r="G38" s="123"/>
-      <c r="H38" s="123"/>
-      <c r="I38" s="123"/>
-      <c r="J38" s="124"/>
+      <c r="G38" s="109"/>
+      <c r="H38" s="109"/>
+      <c r="I38" s="109"/>
+      <c r="J38" s="110"/>
     </row>
     <row r="39" spans="1:10" ht="14">
       <c r="A39" s="35"/>
@@ -14005,18 +14005,18 @@
       <c r="A51" s="5"/>
     </row>
     <row r="52" spans="1:10" ht="21">
-      <c r="A52" s="139" t="s">
+      <c r="A52" s="106" t="s">
         <v>36</v>
       </c>
-      <c r="B52" s="140"/>
-      <c r="C52" s="141"/>
-      <c r="D52" s="141"/>
-      <c r="E52" s="141"/>
-      <c r="F52" s="141"/>
-      <c r="G52" s="141"/>
-      <c r="H52" s="141"/>
-      <c r="I52" s="141"/>
-      <c r="J52" s="141"/>
+      <c r="B52" s="107"/>
+      <c r="C52" s="108"/>
+      <c r="D52" s="108"/>
+      <c r="E52" s="108"/>
+      <c r="F52" s="108"/>
+      <c r="G52" s="108"/>
+      <c r="H52" s="108"/>
+      <c r="I52" s="108"/>
+      <c r="J52" s="108"/>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="70" t="s">
@@ -14260,13 +14260,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="G38:J38"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="G37:J37"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A17:D17"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="G5:J5"/>
@@ -14275,6 +14268,13 @@
     <mergeCell ref="D9:J9"/>
     <mergeCell ref="D10:J10"/>
     <mergeCell ref="D11:G11"/>
+    <mergeCell ref="G38:J38"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:D17"/>
   </mergeCells>
   <phoneticPr fontId="42" type="noConversion"/>
   <hyperlinks>
@@ -14289,6 +14289,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
+      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
+      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A8208FA2715C64A841634F2D9D0061C" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0142632bfc745cbd3590bc04c866e52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3f931156-b907-4802-85d4-da78b74d2c50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="52bad56f1cedf5a7e96bfe3d7dae91ef" ns2:_="">
     <xsd:import namespace="3f931156-b907-4802-85d4-da78b74d2c50"/>
@@ -14461,19 +14473,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
-      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
-      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -14523,16 +14532,17 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDAB445C-65E8-4095-B725-2E676BF1AE69}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14550,28 +14560,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
started fixing xlsx template to improve legal links
</commit_message>
<xml_diff>
--- a/static/template_en.xlsx
+++ b/static/template_en.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tducrot/tdr2d/ovh_pricelist/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7732C7E1-70A7-FB49-AF6D-47237A69CE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370DFC44-15A6-394F-878E-C09872B6A607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10640,6 +10640,7 @@
     <definedName name="Portails" hidden="1">{"' calendrier 2000'!$A$1:$Q$38"}</definedName>
     <definedName name="pp" hidden="1">{#N/A,#N/A,FALSE,"Calc";#N/A,#N/A,FALSE,"Sensitivity";#N/A,#N/A,FALSE,"LT Earn.Dil.";#N/A,#N/A,FALSE,"Dil. AVP"}</definedName>
     <definedName name="Pres" hidden="1">{#N/A,#N/A,TRUE,"Cover sheet";#N/A,#N/A,TRUE,"Summary";#N/A,#N/A,TRUE,"Key Assumptions";#N/A,#N/A,TRUE,"Profit &amp; Loss";#N/A,#N/A,TRUE,"Balance Sheet";#N/A,#N/A,TRUE,"Cashflow";#N/A,#N/A,TRUE,"IRR";#N/A,#N/A,TRUE,"Ratios";#N/A,#N/A,TRUE,"Debt analysis"}</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">quote!$A$1:$J$61</definedName>
     <definedName name="Print_CSC_Report_2" hidden="1">{"CSC_1",#N/A,FALSE,"CSC Outputs";"CSC_2",#N/A,FALSE,"CSC Outputs"}</definedName>
     <definedName name="Print_CSC_Report_3" hidden="1">{"CSC_1",#N/A,FALSE,"CSC Outputs";"CSC_2",#N/A,FALSE,"CSC Outputs"}</definedName>
     <definedName name="print4" hidden="1">{#N/A,#N/A,FALSE,"Operations";#N/A,#N/A,FALSE,"Financials"}</definedName>
@@ -11011,7 +11012,6 @@
     <definedName name="zer" hidden="1">{#N/A,#N/A,FALSE,"Calc";#N/A,#N/A,FALSE,"Sensitivity";#N/A,#N/A,FALSE,"LT Earn.Dil.";#N/A,#N/A,FALSE,"Dil. AVP"}</definedName>
     <definedName name="ZERTRET" hidden="1">#REF!</definedName>
     <definedName name="zezrzrzerz" hidden="1">{"equity comps",#N/A,FALSE,"CS Comps";"equity comps",#N/A,FALSE,"PS Comps";"equity comps",#N/A,FALSE,"GIC_Comps";"equity comps",#N/A,FALSE,"GIC2_Comps"}</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">quote!$A$1:$J$63</definedName>
     <definedName name="zz" hidden="1">{"MARCH",#N/A,FALSE,"CONSO OPEX 5899";"FullOpex",#N/A,FALSE,"CONSO OPEX 5899"}</definedName>
     <definedName name="ZZZ" hidden="1">{#N/A,#N/A,TRUE,"Total Market";#N/A,#N/A,TRUE,"Pricing Table";#N/A,#N/A,TRUE,"Residential Minutes";#N/A,#N/A,TRUE,"Small Bus Minutes";#N/A,#N/A,TRUE,"Medium Bus Minures";#N/A,#N/A,TRUE,"Corporate Min penetration";#N/A,#N/A,TRUE,"Line Penetration";#N/A,#N/A,TRUE,"Direct Line Penetration";#N/A,#N/A,TRUE,"Indirect Lines";#N/A,#N/A,TRUE,"Penetration% by Customer";#N/A,#N/A,TRUE,"Penetration% by Product";#N/A,#N/A,TRUE,"Minutes-Revenue by Product";#N/A,#N/A,TRUE,"Product Minute penetration";#N/A,#N/A,TRUE,"Customer Minutes Penetration"}</definedName>
     <definedName name="ZZZA" hidden="1">{"equity comps",#N/A,FALSE,"CS Comps";"equity comps",#N/A,FALSE,"PS Comps";"equity comps",#N/A,FALSE,"GIC_Comps";"equity comps",#N/A,FALSE,"GIC2_Comps";"debt comps",#N/A,FALSE,"CS Comps";"debt comps",#N/A,FALSE,"PS Comps";"debt comps",#N/A,FALSE,"GIC_Comps";"debt comps",#N/A,FALSE,"GIC2_Comps"}</definedName>
@@ -11034,7 +11034,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t xml:space="preserve">Client : </t>
   </si>
@@ -11188,19 +11188,22 @@
   <si>
     <t>DATA PROCESSING AGREEMENT (DPA) dated on August 09, 2023:</t>
   </si>
+  <si>
+    <t>The Client will, as from the time they are made available by OVHcloud, use all the Services specified in this quote during the COMMIT commitment period (the “Commitment Period”). If, before the end of the Commitment Period, the Client ceases to use all or part of the Services, the Client will pay to OVHcloud the full price of the Services for the entire Commitment Period. The balance must be paid immediately. In consideration of the Client’s commitment, the discount provided for in this quote will apply on the public prices for the duration of the Commitment Period. “Public prices” means the prices as published on the website of OVHcloud at the time of the Order of the Services. The discounted prices are not cumulative with other discounts, rebates or offers available on the website of OVHcloud. The prices of the Services that are subject to the Commitment Period (discounts included) are firm for the entire Commitment Period. However, the prices of the Services may be changed during the Commitment Period in the event of an increase of the electricity cost and/or the price of the Third-Party Products. If the Client continues to use the Services after the end of the Commitment Period or if the Client orders additional Services, the public prices in force as published on the website of OVHcloud will apply.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_ * #,##0.00_)\ &quot;€&quot;_ ;_ * \(#,##0.00\)\ &quot;€&quot;_ ;_ * &quot;-&quot;??_)\ &quot;€&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_)\ &quot;€&quot;_ ;_ * \(#,##0.00\)\ &quot;€&quot;_ ;_ * &quot;-&quot;??_)\ &quot;€&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="44">
+  <fonts count="43">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -11384,13 +11387,6 @@
       <b/>
       <sz val="11"/>
       <color indexed="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color indexed="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -11926,7 +11922,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="21" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -11940,57 +11936,51 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="25" borderId="22" applyBorder="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="42" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="24" borderId="0" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="24" borderId="0" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="27" fillId="24" borderId="0" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="17" xfId="57" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="24" borderId="17" xfId="57" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
@@ -12002,16 +11992,13 @@
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="35" fillId="24" borderId="14" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="34" fillId="24" borderId="14" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="11" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="12" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="27" fillId="24" borderId="13" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -12024,25 +12011,19 @@
     <xf numFmtId="0" fontId="26" fillId="27" borderId="19" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="20" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="20" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="19" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="19" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="13" xfId="57" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="24" borderId="20" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="24" borderId="20" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="4" fillId="24" borderId="20" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12057,19 +12038,19 @@
     <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="14" xfId="47" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="24" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="14" xfId="47" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="24" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="24" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="24" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="22" fillId="24" borderId="14" xfId="56" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="22" fillId="24" borderId="14" xfId="56" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="26" borderId="17" xfId="30" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="26" borderId="17" xfId="30" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="16" xfId="47" applyNumberFormat="1" applyBorder="1"/>
@@ -12088,22 +12069,22 @@
     <xf numFmtId="0" fontId="4" fillId="24" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="24" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="24" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="24" borderId="16" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="27" fillId="24" borderId="14" xfId="56" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="27" fillId="24" borderId="14" xfId="56" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="27" fillId="24" borderId="17" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="27" fillId="24" borderId="17" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="38" fillId="24" borderId="14" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="37" fillId="24" borderId="14" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="27" fillId="24" borderId="12" xfId="56" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="27" fillId="24" borderId="12" xfId="56" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12113,14 +12094,14 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="24" borderId="20" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="24" borderId="19" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="24" borderId="19" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="39" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="40" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="40" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="39" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="47" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -12129,7 +12110,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="57" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="57"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="57"/>
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -12165,11 +12146,11 @@
     <xf numFmtId="0" fontId="26" fillId="27" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="40" fillId="24" borderId="0" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="39" fillId="24" borderId="0" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="20" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="24" borderId="20" xfId="61" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="24" borderId="20" xfId="61" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12178,10 +12159,6 @@
     <xf numFmtId="0" fontId="26" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="10" xfId="56" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -12210,23 +12187,80 @@
     <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="28" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="28" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" xfId="47" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="27" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="43" fillId="24" borderId="14" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="42" fillId="24" borderId="14" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="18" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="20" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="15" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="16" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="20" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="19" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="3" fillId="24" borderId="11" xfId="56" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12265,106 +12299,58 @@
     <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="18" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="20" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="15" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="16" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="20" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="19" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="15" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="16" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="17" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="13" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" xfId="56" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="14" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="62">
     <cellStyle name="%" xfId="48" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20 % - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="2" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="3" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="4" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="5" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="7" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="8" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="9" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="11" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="12" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="13" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="15" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="16" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="17" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="18" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="21" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="22" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="23" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="24" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Avertissement" xfId="25" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Calcul" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Cellule liée" xfId="27" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="31" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Centrify gold" xfId="49" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Entrée" xfId="29" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="42" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="61" builtinId="4"/>
     <cellStyle name="Euro" xfId="30" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
     <cellStyle name="Euro 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
     <cellStyle name="Euro 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Insatisfaisant" xfId="31" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Lien hypertexte" xfId="57" builtinId="8"/>
+    <cellStyle name="Explanatory Text" xfId="35" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="33" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="37" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="38" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="39" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="40" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8"/>
+    <cellStyle name="Input" xfId="29" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Milliers 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
     <cellStyle name="Milliers 3" xfId="52" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
     <cellStyle name="Milliers 4" xfId="59" xr:uid="{14D347B5-402F-8D41-8897-7199A386B517}"/>
-    <cellStyle name="Monétaire" xfId="61" builtinId="4"/>
     <cellStyle name="Monétaire 2" xfId="46" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Neutre" xfId="32" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="32" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
     <cellStyle name="Normal 2 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
@@ -12372,20 +12358,14 @@
     <cellStyle name="Normal 2 3 2" xfId="58" xr:uid="{86FC485C-AE2B-AF43-ADC9-8C2E482CE86C}"/>
     <cellStyle name="Normal 3" xfId="45" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
     <cellStyle name="Note" xfId="28" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="34" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Pourcentage 2" xfId="53" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
     <cellStyle name="Pourcentage 2 2" xfId="54" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
     <cellStyle name="Pourcentage 3" xfId="55" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
     <cellStyle name="Pourcentage 4" xfId="60" xr:uid="{22625C26-9810-C74D-A5AA-B84EE3F92A6B}"/>
-    <cellStyle name="Satisfaisant" xfId="33" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Sortie" xfId="34" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texte explicatif" xfId="35" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Titre" xfId="36" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Titre 1" xfId="37" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Titre 2" xfId="38" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Titre 3" xfId="39" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Titre 4" xfId="40" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="36" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Vérification" xfId="42" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="25" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -12753,10 +12733,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J106"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -13342,258 +13322,258 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="64"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="22"/>
+      <c r="A1" s="59"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10" ht="20">
-      <c r="A2" s="139" t="s">
+      <c r="A2" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="140"/>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="140"/>
-      <c r="F2" s="140"/>
-      <c r="G2" s="140"/>
-      <c r="H2" s="140"/>
-      <c r="I2" s="140"/>
-      <c r="J2" s="141"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="104"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="65"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="24"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="22"/>
     </row>
     <row r="5" spans="1:10" ht="14">
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="98"/>
-      <c r="G5" s="111">
+      <c r="F5" s="91"/>
+      <c r="G5" s="123">
         <f ca="1">NOW()</f>
-        <v>45196.822671759262</v>
+        <v>45321.718458680552</v>
       </c>
-      <c r="H5" s="111"/>
-      <c r="I5" s="111"/>
-      <c r="J5" s="112"/>
+      <c r="H5" s="123"/>
+      <c r="I5" s="123"/>
+      <c r="J5" s="124"/>
     </row>
     <row r="6" spans="1:10" ht="55" customHeight="1">
-      <c r="B6" s="103" t="s">
+      <c r="B6" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="66" t="s">
+      <c r="C6" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="99" t="s">
+      <c r="E6" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="96"/>
-      <c r="J6" s="100"/>
+      <c r="F6" s="89"/>
+      <c r="J6" s="93"/>
     </row>
     <row r="7" spans="1:10" ht="14">
-      <c r="A7" s="74"/>
-      <c r="B7" s="95"/>
-      <c r="C7" s="67" t="s">
+      <c r="A7" s="69"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="101" t="s">
+      <c r="E7" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="102"/>
-      <c r="G7" s="113"/>
-      <c r="H7" s="113"/>
-      <c r="I7" s="113"/>
-      <c r="J7" s="114"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
+      <c r="J7" s="126"/>
     </row>
     <row r="8" spans="1:10" ht="14">
-      <c r="C8" s="67">
+      <c r="C8" s="62">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="6" customFormat="1" ht="14">
-      <c r="A9" s="115" t="s">
+      <c r="A9" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="116"/>
-      <c r="C9" s="68" t="s">
+      <c r="B9" s="128"/>
+      <c r="C9" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="115" t="s">
+      <c r="D9" s="127" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="117"/>
-      <c r="F9" s="117"/>
-      <c r="G9" s="117"/>
-      <c r="H9" s="117"/>
-      <c r="I9" s="117"/>
-      <c r="J9" s="116"/>
+      <c r="E9" s="129"/>
+      <c r="F9" s="129"/>
+      <c r="G9" s="129"/>
+      <c r="H9" s="129"/>
+      <c r="I9" s="129"/>
+      <c r="J9" s="128"/>
     </row>
     <row r="10" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="87">
+      <c r="B10" s="56"/>
+      <c r="C10" s="82">
         <v>10</v>
       </c>
-      <c r="D10" s="118" t="s">
+      <c r="D10" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="119"/>
-      <c r="F10" s="119"/>
-      <c r="G10" s="119"/>
-      <c r="H10" s="119"/>
-      <c r="I10" s="119"/>
-      <c r="J10" s="120"/>
+      <c r="E10" s="131"/>
+      <c r="F10" s="131"/>
+      <c r="G10" s="131"/>
+      <c r="H10" s="131"/>
+      <c r="I10" s="131"/>
+      <c r="J10" s="132"/>
     </row>
     <row r="11" spans="1:10" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="87">
+      <c r="B11" s="33"/>
+      <c r="C11" s="82">
         <v>250</v>
       </c>
-      <c r="D11" s="121"/>
-      <c r="E11" s="122"/>
-      <c r="F11" s="122"/>
-      <c r="G11" s="122"/>
-      <c r="H11" s="39"/>
-      <c r="J11" s="8"/>
+      <c r="D11" s="133"/>
+      <c r="E11" s="134"/>
+      <c r="F11" s="134"/>
+      <c r="G11" s="134"/>
+      <c r="H11" s="34"/>
+      <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="87">
+      <c r="B12" s="36"/>
+      <c r="C12" s="82">
         <v>0</v>
       </c>
-      <c r="D12" s="109"/>
-      <c r="E12" s="110"/>
-      <c r="F12" s="110"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="15"/>
+      <c r="D12" s="121"/>
+      <c r="E12" s="122"/>
+      <c r="F12" s="122"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="13"/>
     </row>
     <row r="13" spans="1:10" s="6" customFormat="1" ht="15" customHeight="1">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="87">
+      <c r="B13" s="14"/>
+      <c r="C13" s="82">
         <v>12</v>
       </c>
-      <c r="D13" s="127"/>
-      <c r="E13" s="128"/>
-      <c r="F13" s="128"/>
-      <c r="G13" s="128"/>
-      <c r="H13" s="128"/>
-      <c r="I13" s="128"/>
-      <c r="J13" s="129"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="110"/>
+      <c r="G13" s="110"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="110"/>
+      <c r="J13" s="111"/>
     </row>
     <row r="15" spans="1:10" s="6" customFormat="1" ht="73.5" customHeight="1">
-      <c r="A15" s="134" t="s">
+      <c r="A15" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="135"/>
-      <c r="C15" s="135"/>
-      <c r="D15" s="136"/>
-      <c r="E15" s="49" t="s">
+      <c r="B15" s="117"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="18" t="str">
+      <c r="F15" s="16" t="str">
         <f>"Unit Price "&amp;C5&amp;" ex. VAT/month"</f>
         <v>Unit Price € ex. VAT/month</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="I15" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="18" t="str">
+      <c r="J15" s="16" t="str">
         <f>"Price "&amp;C5&amp;" ex. VAT/month"</f>
         <v>Price € ex. VAT/month</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1">
-      <c r="A16" s="130" t="s">
+      <c r="A16" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="131"/>
-      <c r="C16" s="131"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="132"/>
-      <c r="F16" s="132"/>
-      <c r="G16" s="132"/>
-      <c r="H16" s="132"/>
-      <c r="I16" s="132"/>
-      <c r="J16" s="133"/>
+      <c r="B16" s="113"/>
+      <c r="C16" s="113"/>
+      <c r="D16" s="113"/>
+      <c r="E16" s="114"/>
+      <c r="F16" s="114"/>
+      <c r="G16" s="114"/>
+      <c r="H16" s="114"/>
+      <c r="I16" s="114"/>
+      <c r="J16" s="115"/>
     </row>
     <row r="17" spans="1:10" ht="122" customHeight="1">
-      <c r="A17" s="137" t="s">
+      <c r="A17" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="138"/>
-      <c r="C17" s="138"/>
-      <c r="D17" s="138"/>
-      <c r="E17" s="33">
+      <c r="B17" s="120"/>
+      <c r="C17" s="120"/>
+      <c r="D17" s="120"/>
+      <c r="E17" s="29">
         <v>10</v>
       </c>
-      <c r="F17" s="89">
+      <c r="F17" s="84">
         <v>3109</v>
       </c>
-      <c r="G17" s="34">
+      <c r="G17" s="30">
         <v>1</v>
       </c>
-      <c r="H17" s="88">
+      <c r="H17" s="83">
         <v>36</v>
       </c>
-      <c r="I17" s="62">
+      <c r="I17" s="57">
         <v>0.15</v>
       </c>
-      <c r="J17" s="63">
+      <c r="J17" s="58">
         <f>F17*G17*(1-I17)</f>
         <v>2642.65</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="14">
-      <c r="A18" s="50"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="47"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
-      <c r="A19" s="44"/>
+      <c r="A19" s="39"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -13604,190 +13584,190 @@
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
-      <c r="A20" s="11"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="2"/>
-      <c r="D20" s="81" t="s">
+      <c r="D20" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="82"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="59">
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="77"/>
+      <c r="I20" s="77"/>
+      <c r="J20" s="54">
         <f>SUM(J17:J17)</f>
         <v>2642.65</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="D21" s="83" t="str">
+      <c r="A21" s="10"/>
+      <c r="D21" s="78" t="str">
         <f>C9&amp;" SUPPORT  ("&amp;C10&amp;"% Minimum " &amp; C11&amp;")"</f>
         <v>BUSINESS SUPPORT  (10% Minimum 250)</v>
       </c>
-      <c r="E21" s="107"/>
-      <c r="F21" s="107"/>
-      <c r="G21" s="107"/>
-      <c r="H21" s="107"/>
-      <c r="I21" s="107"/>
-      <c r="J21" s="56">
+      <c r="E21" s="100"/>
+      <c r="F21" s="100"/>
+      <c r="G21" s="100"/>
+      <c r="H21" s="100"/>
+      <c r="I21" s="100"/>
+      <c r="J21" s="51">
         <f>MAX(0.01*$C$10*J20,$C$11)</f>
         <v>264.26500000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="19" customFormat="1" ht="18" customHeight="1">
-      <c r="A22" s="11"/>
+    <row r="22" spans="1:10" s="17" customFormat="1" ht="18" customHeight="1">
+      <c r="A22" s="10"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="83" t="str">
+      <c r="D22" s="78" t="str">
         <f>IF(C12&gt;0,"Exceptional Discount (-"&amp;C12&amp;"%)","")</f>
         <v/>
       </c>
-      <c r="E22" s="107"/>
-      <c r="F22" s="107"/>
-      <c r="G22" s="107"/>
-      <c r="H22" s="107"/>
-      <c r="I22" s="107"/>
-      <c r="J22" s="56">
+      <c r="E22" s="100"/>
+      <c r="F22" s="100"/>
+      <c r="G22" s="100"/>
+      <c r="H22" s="100"/>
+      <c r="I22" s="100"/>
+      <c r="J22" s="51">
         <f>(0-J20-J21)*($C$12/100)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="16" customHeight="1">
-      <c r="A23" s="11"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="83" t="str">
+      <c r="D23" s="78" t="str">
         <f>"MONTHLY COST ex. VAT with SUPPORT in "&amp;C6</f>
         <v>MONTHLY COST ex. VAT with SUPPORT in EURO</v>
       </c>
-      <c r="E23" s="107"/>
-      <c r="F23" s="107"/>
-      <c r="G23" s="107"/>
-      <c r="H23" s="107"/>
-      <c r="I23" s="107"/>
-      <c r="J23" s="58">
+      <c r="E23" s="100"/>
+      <c r="F23" s="100"/>
+      <c r="G23" s="100"/>
+      <c r="H23" s="100"/>
+      <c r="I23" s="100"/>
+      <c r="J23" s="53">
         <f>J20+J21+J22</f>
         <v>2906.915</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="16" customHeight="1">
-      <c r="A24" s="11"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
-      <c r="D24" s="83" t="str">
+      <c r="D24" s="78" t="str">
         <f>"VAT ("&amp;$C$8&amp;"%)"</f>
         <v>VAT (20%)</v>
       </c>
-      <c r="E24" s="107"/>
-      <c r="F24" s="107"/>
-      <c r="G24" s="107"/>
-      <c r="H24" s="107"/>
-      <c r="I24" s="107"/>
-      <c r="J24" s="108">
+      <c r="E24" s="100"/>
+      <c r="F24" s="100"/>
+      <c r="G24" s="100"/>
+      <c r="H24" s="100"/>
+      <c r="I24" s="100"/>
+      <c r="J24" s="101">
         <f>$C$8*J23/100</f>
         <v>581.38300000000004</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="14" customHeight="1">
-      <c r="A25" s="11"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="83" t="s">
+      <c r="D25" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="107"/>
-      <c r="F25" s="107"/>
-      <c r="G25" s="107"/>
-      <c r="H25" s="107"/>
-      <c r="I25" s="107"/>
-      <c r="J25" s="20">
+      <c r="E25" s="100"/>
+      <c r="F25" s="100"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="100"/>
+      <c r="I25" s="100"/>
+      <c r="J25" s="18">
         <f>SUM(E17:E18)</f>
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="14" customHeight="1">
-      <c r="A26" s="11"/>
+      <c r="A26" s="10"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
-      <c r="D26" s="83"/>
-      <c r="E26" s="107"/>
-      <c r="F26" s="107"/>
-      <c r="G26" s="107"/>
-      <c r="H26" s="107"/>
-      <c r="I26" s="107"/>
-      <c r="J26" s="20"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="100"/>
+      <c r="F26" s="100"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="100"/>
+      <c r="I26" s="100"/>
+      <c r="J26" s="18"/>
     </row>
     <row r="27" spans="1:10" s="6" customFormat="1" ht="16" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="D27" s="83" t="str">
+      <c r="A27" s="10"/>
+      <c r="D27" s="78" t="str">
         <f>"Monthly COST including VAT and SUPPORT in "&amp;C6</f>
         <v>Monthly COST including VAT and SUPPORT in EURO</v>
       </c>
-      <c r="E27" s="107"/>
-      <c r="F27" s="107"/>
-      <c r="G27" s="107"/>
-      <c r="H27" s="107"/>
-      <c r="I27" s="107"/>
-      <c r="J27" s="56">
+      <c r="E27" s="100"/>
+      <c r="F27" s="100"/>
+      <c r="G27" s="100"/>
+      <c r="H27" s="100"/>
+      <c r="I27" s="100"/>
+      <c r="J27" s="51">
         <f>J23*(1+$C$8/100)</f>
         <v>3488.2979999999998</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
-      <c r="A28" s="11"/>
-      <c r="D28" s="83" t="str">
+      <c r="A28" s="10"/>
+      <c r="D28" s="78" t="str">
         <f>"Setup Fees including VAT in "&amp;C6</f>
         <v>Setup Fees including VAT in EURO</v>
       </c>
-      <c r="E28" s="107"/>
-      <c r="F28" s="107"/>
-      <c r="G28" s="107"/>
-      <c r="H28" s="107"/>
-      <c r="I28" s="107"/>
-      <c r="J28" s="56">
+      <c r="E28" s="100"/>
+      <c r="F28" s="100"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="100"/>
+      <c r="I28" s="100"/>
+      <c r="J28" s="51">
         <f>J25*(1+$C$8/100)</f>
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="6" customFormat="1" ht="14" customHeight="1">
-      <c r="A29" s="11"/>
-      <c r="D29" s="83" t="str">
+      <c r="A29" s="10"/>
+      <c r="D29" s="78" t="str">
         <f>"BUDGET in "&amp;C6&amp;" ex. VAT ("&amp;$C$13&amp;" Months)"</f>
         <v>BUDGET in EURO ex. VAT (12 Months)</v>
       </c>
-      <c r="E29" s="107"/>
-      <c r="F29" s="107"/>
-      <c r="G29" s="107"/>
-      <c r="H29" s="107"/>
-      <c r="I29" s="107"/>
-      <c r="J29" s="45">
+      <c r="E29" s="100"/>
+      <c r="F29" s="100"/>
+      <c r="G29" s="100"/>
+      <c r="H29" s="100"/>
+      <c r="I29" s="100"/>
+      <c r="J29" s="40">
         <f>J23*$C$13+J25</f>
         <v>34892.979999999996</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="6" customFormat="1" ht="15.5" customHeight="1">
-      <c r="A30" s="11"/>
-      <c r="D30" s="85" t="str">
+      <c r="A30" s="10"/>
+      <c r="D30" s="80" t="str">
         <f>"BUDGET in "&amp;C6&amp;" including VAT ("&amp;$C$13&amp;" Months) - "&amp;$C$7&amp;" "&amp;$C$8&amp;"%"</f>
         <v>BUDGET in EURO including VAT (12 Months) - TVA 20%</v>
       </c>
-      <c r="E30" s="86"/>
-      <c r="F30" s="86"/>
-      <c r="G30" s="86"/>
-      <c r="H30" s="86"/>
-      <c r="I30" s="86"/>
-      <c r="J30" s="57">
+      <c r="E30" s="81"/>
+      <c r="F30" s="81"/>
+      <c r="G30" s="81"/>
+      <c r="H30" s="81"/>
+      <c r="I30" s="81"/>
+      <c r="J30" s="52">
         <f>J29*1.2</f>
         <v>41871.575999999994</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="14">
-      <c r="A31" s="11"/>
+      <c r="A31" s="10"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
     </row>
     <row r="32" spans="1:10" s="6" customFormat="1" ht="14">
-      <c r="A32" s="46"/>
+      <c r="A32" s="41"/>
       <c r="C32" s="1"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -13798,507 +13778,489 @@
       <c r="J32" s="4"/>
     </row>
     <row r="33" spans="1:10" ht="14">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="29"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="26"/>
     </row>
     <row r="34" spans="1:10" ht="14">
-      <c r="A34" s="125"/>
-      <c r="B34" s="126"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="31"/>
+      <c r="A34" s="107"/>
+      <c r="B34" s="108"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="27"/>
+      <c r="J34" s="28"/>
     </row>
     <row r="35" spans="1:10" ht="15">
-      <c r="A35" s="75"/>
-      <c r="B35" s="75" t="s">
+      <c r="A35" s="70"/>
+      <c r="B35" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="77" t="s">
+      <c r="C35" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="D35" s="77"/>
-      <c r="E35" s="77"/>
-      <c r="F35" s="77"/>
-      <c r="G35" s="77"/>
-      <c r="H35" s="77"/>
-      <c r="I35" s="77"/>
-      <c r="J35" s="78"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="72"/>
+      <c r="I35" s="72"/>
+      <c r="J35" s="73"/>
     </row>
     <row r="36" spans="1:10" ht="15">
-      <c r="A36" s="76"/>
-      <c r="B36" s="76" t="s">
+      <c r="A36" s="71"/>
+      <c r="B36" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="77" t="s">
+      <c r="C36" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="D36" s="77"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="77"/>
-      <c r="G36" s="77"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="77"/>
-      <c r="J36" s="78"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="72"/>
+      <c r="H36" s="72"/>
+      <c r="I36" s="72"/>
+      <c r="J36" s="73"/>
     </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="93"/>
+    <row r="37" spans="1:10" ht="15">
+      <c r="A37" s="71"/>
+      <c r="B37" s="71" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="72" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="72"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="72"/>
+      <c r="H37" s="72"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="73"/>
     </row>
-    <row r="38" spans="1:10" ht="15">
-      <c r="A38" s="90"/>
-      <c r="B38" s="91"/>
+    <row r="38" spans="1:10" ht="14">
+      <c r="A38" s="85"/>
+      <c r="B38" s="86"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="79" t="s">
+    </row>
+    <row r="39" spans="1:10" ht="21">
+      <c r="A39" s="97" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="98"/>
+      <c r="C39" s="99"/>
+      <c r="D39" s="99"/>
+      <c r="E39" s="99"/>
+      <c r="F39" s="99"/>
+      <c r="G39" s="99"/>
+      <c r="H39" s="99"/>
+      <c r="I39" s="99"/>
+      <c r="J39" s="99"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="64" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="37"/>
+      <c r="C40" s="38"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="65" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" s="37"/>
+      <c r="C41" s="38"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="65"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="38"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="66" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="37"/>
+      <c r="C43" s="38"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="68" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" s="37"/>
+      <c r="C44" s="38"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="67" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="37"/>
+      <c r="C45" s="38"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="68" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="37"/>
+      <c r="C46" s="38"/>
+    </row>
+    <row r="47" spans="1:10" ht="14">
+      <c r="A47" s="85"/>
+      <c r="B47" s="86"/>
+      <c r="C47" s="34"/>
+    </row>
+    <row r="48" spans="1:10" ht="91" customHeight="1">
+      <c r="A48" s="135" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48" s="135"/>
+      <c r="C48" s="135"/>
+      <c r="D48" s="135"/>
+      <c r="E48" s="135"/>
+      <c r="F48" s="135"/>
+      <c r="G48" s="135"/>
+      <c r="H48" s="135"/>
+      <c r="I48" s="135"/>
+      <c r="J48" s="135"/>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="87"/>
+      <c r="C49" s="23"/>
+    </row>
+    <row r="50" spans="1:10" ht="15">
+      <c r="A50" s="5"/>
+      <c r="B50" s="23"/>
+      <c r="D50" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="E38" s="80"/>
-      <c r="F38" s="80"/>
-      <c r="G38" s="80"/>
-      <c r="H38" s="80"/>
-      <c r="I38" s="80"/>
-      <c r="J38" s="84"/>
+      <c r="E50" s="75"/>
+      <c r="F50" s="75"/>
+      <c r="G50" s="75"/>
+      <c r="H50" s="75"/>
+      <c r="I50" s="75"/>
+      <c r="J50" s="79"/>
     </row>
-    <row r="39" spans="1:10" ht="14">
-      <c r="A39" s="37"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="11" t="s">
+    <row r="51" spans="1:10" ht="14">
+      <c r="A51" s="5"/>
+      <c r="D51" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="123"/>
-      <c r="H39" s="123"/>
-      <c r="I39" s="123"/>
-      <c r="J39" s="124"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="105"/>
+      <c r="H51" s="105"/>
+      <c r="I51" s="105"/>
+      <c r="J51" s="106"/>
     </row>
-    <row r="40" spans="1:10" ht="14">
-      <c r="A40" s="37"/>
-      <c r="B40" s="39"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="5"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="123"/>
-      <c r="H40" s="123"/>
-      <c r="I40" s="123"/>
-      <c r="J40" s="124"/>
+    <row r="52" spans="1:10" ht="14">
+      <c r="D52" s="5"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="105"/>
+      <c r="I52" s="105"/>
+      <c r="J52" s="106"/>
     </row>
-    <row r="41" spans="1:10" ht="14">
-      <c r="A41" s="35"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="11" t="s">
+    <row r="53" spans="1:10" ht="14">
+      <c r="D53" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="8"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="7"/>
     </row>
-    <row r="42" spans="1:10" ht="14">
-      <c r="A42" s="32"/>
-      <c r="B42" s="92"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="8"/>
+    <row r="54" spans="1:10" ht="14">
+      <c r="D54" s="10"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="7"/>
     </row>
-    <row r="43" spans="1:10" ht="14">
-      <c r="A43" s="37"/>
-      <c r="B43" s="39"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="14" t="s">
+    <row r="55" spans="1:10" ht="14">
+      <c r="D55" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="17"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="8"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="7"/>
     </row>
-    <row r="44" spans="1:10" ht="14">
-      <c r="A44" s="25"/>
-      <c r="B44" s="39"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="8"/>
+    <row r="56" spans="1:10" ht="14">
+      <c r="D56" s="12"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="7"/>
     </row>
-    <row r="45" spans="1:10" ht="14">
-      <c r="A45" s="90"/>
-      <c r="B45" s="91"/>
-      <c r="C45" s="39"/>
-      <c r="D45" s="11" t="s">
+    <row r="57" spans="1:10" ht="14">
+      <c r="D57" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="8"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="7"/>
     </row>
-    <row r="46" spans="1:10" ht="14">
-      <c r="A46" s="90"/>
-      <c r="B46" s="91"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="8"/>
+    <row r="58" spans="1:10" ht="14">
+      <c r="D58" s="10"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="7"/>
     </row>
-    <row r="47" spans="1:10" ht="14">
-      <c r="A47" s="90"/>
-      <c r="B47" s="91"/>
-      <c r="C47" s="39"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="8"/>
+    <row r="59" spans="1:10" ht="14">
+      <c r="D59" s="10"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="7"/>
     </row>
-    <row r="48" spans="1:10" ht="14">
-      <c r="A48" s="90"/>
-      <c r="B48" s="91"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="8"/>
+    <row r="60" spans="1:10" ht="14">
+      <c r="A60" s="66"/>
+      <c r="B60" s="37"/>
+      <c r="C60" s="38"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="7"/>
     </row>
-    <row r="49" spans="1:10" ht="14">
-      <c r="A49" s="90"/>
-      <c r="B49" s="91"/>
-      <c r="C49" s="39"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="8"/>
+    <row r="61" spans="1:10" ht="14">
+      <c r="A61" s="68"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="7"/>
     </row>
-    <row r="50" spans="1:10" ht="14">
-      <c r="A50" s="90"/>
-      <c r="B50" s="91"/>
-      <c r="C50" s="39"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="10"/>
+    <row r="62" spans="1:10" ht="14">
+      <c r="A62" s="67"/>
+      <c r="B62" s="37"/>
+      <c r="C62" s="38"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="8"/>
+      <c r="F62" s="8"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="9"/>
     </row>
-    <row r="51" spans="1:10">
-      <c r="A51" s="94"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="1" t="s">
+    <row r="63" spans="1:10">
+      <c r="A63" s="68"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="38"/>
+      <c r="D63" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
-      <c r="A52" s="5"/>
-      <c r="B52" s="26"/>
-    </row>
-    <row r="53" spans="1:10">
-      <c r="A53" s="5"/>
-    </row>
-    <row r="54" spans="1:10" ht="21">
-      <c r="A54" s="104" t="s">
-        <v>36</v>
-      </c>
-      <c r="B54" s="105"/>
-      <c r="C54" s="106"/>
-      <c r="D54" s="106"/>
-      <c r="E54" s="106"/>
-      <c r="F54" s="106"/>
-      <c r="G54" s="106"/>
-      <c r="H54" s="106"/>
-      <c r="I54" s="106"/>
-      <c r="J54" s="106"/>
-    </row>
-    <row r="55" spans="1:10">
-      <c r="A55" s="69" t="s">
-        <v>38</v>
-      </c>
-      <c r="B55" s="42"/>
-      <c r="C55" s="43"/>
-    </row>
-    <row r="56" spans="1:10">
-      <c r="A56" s="70" t="s">
-        <v>37</v>
-      </c>
-      <c r="B56" s="42"/>
-      <c r="C56" s="43"/>
-    </row>
-    <row r="57" spans="1:10">
-      <c r="A57" s="70"/>
-      <c r="B57" s="42"/>
-      <c r="C57" s="43"/>
-    </row>
-    <row r="58" spans="1:10">
-      <c r="A58" s="71" t="s">
-        <v>42</v>
-      </c>
-      <c r="B58" s="42"/>
-      <c r="C58" s="43"/>
-    </row>
-    <row r="59" spans="1:10">
-      <c r="A59" s="73" t="s">
-        <v>39</v>
-      </c>
-      <c r="B59" s="42"/>
-      <c r="C59" s="43"/>
-    </row>
-    <row r="60" spans="1:10">
-      <c r="A60" s="72" t="s">
-        <v>41</v>
-      </c>
-      <c r="B60" s="42"/>
-      <c r="C60" s="43"/>
-    </row>
-    <row r="61" spans="1:10">
-      <c r="A61" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="B61" s="42"/>
-      <c r="C61" s="43"/>
-    </row>
-    <row r="62" spans="1:10">
-      <c r="A62" s="71"/>
-      <c r="B62" s="42"/>
-      <c r="C62" s="43"/>
-    </row>
-    <row r="63" spans="1:10">
-      <c r="A63" s="73"/>
-      <c r="B63" s="42"/>
-      <c r="C63" s="43"/>
-    </row>
     <row r="64" spans="1:10">
-      <c r="A64" s="72"/>
-      <c r="B64" s="42"/>
-      <c r="C64" s="43"/>
+      <c r="A64" s="66"/>
+      <c r="B64" s="37"/>
+      <c r="C64" s="38"/>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="73"/>
-      <c r="B65" s="42"/>
-      <c r="C65" s="43"/>
+      <c r="A65" s="68"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="38"/>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="71"/>
-      <c r="B66" s="42"/>
-      <c r="C66" s="43"/>
+      <c r="A66" s="67"/>
+      <c r="B66" s="37"/>
+      <c r="C66" s="38"/>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="73"/>
-      <c r="B67" s="42"/>
-      <c r="C67" s="43"/>
+      <c r="A67" s="68"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="38"/>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="72"/>
-      <c r="B68" s="42"/>
-      <c r="C68" s="43"/>
+      <c r="A68" s="66"/>
+      <c r="B68" s="37"/>
+      <c r="C68" s="38"/>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="73"/>
-      <c r="B69" s="42"/>
-      <c r="C69" s="43"/>
+      <c r="A69" s="68"/>
+      <c r="B69" s="37"/>
+      <c r="C69" s="38"/>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="71"/>
-      <c r="B70" s="42"/>
-      <c r="C70" s="43"/>
+      <c r="A70" s="67"/>
+      <c r="B70" s="37"/>
+      <c r="C70" s="38"/>
     </row>
     <row r="71" spans="1:3">
-      <c r="A71" s="73"/>
-      <c r="B71" s="42"/>
-      <c r="C71" s="43"/>
+      <c r="A71" s="68"/>
+      <c r="B71" s="37"/>
+      <c r="C71" s="38"/>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="72"/>
-      <c r="B72" s="42"/>
-      <c r="C72" s="43"/>
+      <c r="A72" s="66"/>
+      <c r="B72" s="37"/>
+      <c r="C72" s="38"/>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="73"/>
-      <c r="B73" s="42"/>
-      <c r="C73" s="43"/>
+      <c r="A73" s="68"/>
+      <c r="B73" s="37"/>
+      <c r="C73" s="38"/>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="71"/>
-      <c r="B74" s="42"/>
-      <c r="C74" s="43"/>
+      <c r="A74" s="67"/>
+      <c r="B74" s="37"/>
+      <c r="C74" s="38"/>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="73"/>
-      <c r="B75" s="42"/>
-      <c r="C75" s="43"/>
+      <c r="A75" s="68"/>
+      <c r="B75" s="37"/>
+      <c r="C75" s="38"/>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="72"/>
-      <c r="B76" s="42"/>
-      <c r="C76" s="43"/>
+      <c r="A76" s="66"/>
+      <c r="B76" s="37"/>
+      <c r="C76" s="38"/>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="73"/>
-      <c r="B77" s="42"/>
-      <c r="C77" s="43"/>
+      <c r="A77" s="68"/>
+      <c r="B77" s="37"/>
+      <c r="C77" s="38"/>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="71"/>
-      <c r="B78" s="42"/>
-      <c r="C78" s="43"/>
+      <c r="A78" s="67"/>
+      <c r="B78" s="37"/>
+      <c r="C78" s="38"/>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="73"/>
-      <c r="B79" s="42"/>
-      <c r="C79" s="43"/>
+      <c r="A79" s="68"/>
+      <c r="B79" s="37"/>
+      <c r="C79" s="38"/>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="72"/>
-      <c r="B80" s="42"/>
-      <c r="C80" s="43"/>
+      <c r="A80" s="66"/>
+      <c r="B80" s="37"/>
+      <c r="C80" s="38"/>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="73"/>
-      <c r="B81" s="42"/>
-      <c r="C81" s="43"/>
+      <c r="A81" s="68"/>
+      <c r="B81" s="37"/>
+      <c r="C81" s="38"/>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="71"/>
-      <c r="B82" s="42"/>
-      <c r="C82" s="43"/>
+      <c r="A82" s="67"/>
+      <c r="B82" s="37"/>
+      <c r="C82" s="38"/>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="73"/>
-      <c r="B83" s="42"/>
-      <c r="C83" s="43"/>
+      <c r="A83" s="68"/>
+      <c r="B83" s="37"/>
+      <c r="C83" s="38"/>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="72"/>
-      <c r="B84" s="42"/>
-      <c r="C84" s="43"/>
+      <c r="A84" s="66"/>
+      <c r="B84" s="37"/>
+      <c r="C84" s="38"/>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="73"/>
-      <c r="B85" s="42"/>
-      <c r="C85" s="43"/>
+      <c r="A85" s="68"/>
+      <c r="B85" s="37"/>
+      <c r="C85" s="38"/>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="71"/>
-      <c r="B86" s="42"/>
-      <c r="C86" s="43"/>
+      <c r="A86" s="67"/>
+      <c r="B86" s="37"/>
+      <c r="C86" s="38"/>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="73"/>
-      <c r="B87" s="42"/>
-      <c r="C87" s="43"/>
+      <c r="A87" s="68"/>
+      <c r="B87" s="37"/>
+      <c r="C87" s="38"/>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="72"/>
-      <c r="B88" s="42"/>
-      <c r="C88" s="43"/>
+      <c r="A88" s="66"/>
+      <c r="B88" s="37"/>
+      <c r="C88" s="38"/>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="73"/>
-      <c r="B89" s="42"/>
-      <c r="C89" s="43"/>
+      <c r="A89" s="68"/>
     </row>
     <row r="90" spans="1:3">
-      <c r="A90" s="71"/>
-      <c r="B90" s="42"/>
-      <c r="C90" s="43"/>
+      <c r="A90" s="67"/>
     </row>
-    <row r="91" spans="1:3">
-      <c r="A91" s="73"/>
+    <row r="91" spans="1:3" ht="15" customHeight="1">
+      <c r="A91" s="68"/>
     </row>
-    <row r="92" spans="1:3">
-      <c r="A92" s="72"/>
+    <row r="92" spans="1:3" ht="15" customHeight="1">
+      <c r="A92" s="66"/>
     </row>
-    <row r="93" spans="1:3" ht="15" customHeight="1">
-      <c r="A93" s="73"/>
+    <row r="93" spans="1:3">
+      <c r="A93" s="68"/>
     </row>
-    <row r="94" spans="1:3" ht="15" customHeight="1">
-      <c r="A94" s="71"/>
+    <row r="94" spans="1:3" ht="16" customHeight="1">
+      <c r="A94" s="67"/>
     </row>
-    <row r="95" spans="1:3">
-      <c r="A95" s="73"/>
+    <row r="95" spans="1:3" ht="15" customHeight="1">
+      <c r="A95" s="68"/>
     </row>
-    <row r="96" spans="1:3" ht="16" customHeight="1">
-      <c r="A96" s="72"/>
+    <row r="96" spans="1:3" ht="15" customHeight="1">
+      <c r="A96" s="66"/>
     </row>
     <row r="97" spans="1:1" ht="15" customHeight="1">
-      <c r="A97" s="73"/>
+      <c r="A97" s="68"/>
     </row>
     <row r="98" spans="1:1" ht="15" customHeight="1">
-      <c r="A98" s="71"/>
+      <c r="A98" s="67"/>
     </row>
     <row r="99" spans="1:1" ht="15" customHeight="1">
-      <c r="A99" s="73"/>
+      <c r="A99" s="68"/>
     </row>
-    <row r="100" spans="1:1" ht="15" customHeight="1">
-      <c r="A100" s="72"/>
+    <row r="100" spans="1:1">
+      <c r="A100" s="66"/>
     </row>
-    <row r="101" spans="1:1" ht="15" customHeight="1">
-      <c r="A101" s="73"/>
+    <row r="101" spans="1:1">
+      <c r="A101" s="68"/>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="71"/>
+      <c r="A102" s="67"/>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="73"/>
+      <c r="A103" s="68"/>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104" s="72"/>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" s="73"/>
-    </row>
-    <row r="106" spans="1:1">
-      <c r="A106" s="71"/>
+      <c r="A104" s="66"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="G40:J40"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="G39:J39"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A17:D17"/>
+  <mergeCells count="15">
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="G7:J7"/>
@@ -14306,11 +14268,19 @@
     <mergeCell ref="D9:J9"/>
     <mergeCell ref="D10:J10"/>
     <mergeCell ref="D11:G11"/>
+    <mergeCell ref="G52:J52"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="G51:J51"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A48:J48"/>
   </mergeCells>
-  <phoneticPr fontId="41" type="noConversion"/>
+  <phoneticPr fontId="40" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A61" r:id="rId1" xr:uid="{30AE7B39-CB55-6143-880E-9274BFAE3726}"/>
-    <hyperlink ref="A59" r:id="rId2" xr:uid="{090F80D4-B20B-F74A-A0D7-1E595C457070}"/>
+    <hyperlink ref="A46" r:id="rId1" xr:uid="{30AE7B39-CB55-6143-880E-9274BFAE3726}"/>
+    <hyperlink ref="A44" r:id="rId2" xr:uid="{090F80D4-B20B-F74A-A0D7-1E595C457070}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -14320,6 +14290,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -14369,16 +14348,19 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
+      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
+      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009A8208FA2715C64A841634F2D9D0061C" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e0142632bfc745cbd3590bc04c866e52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3f931156-b907-4802-85d4-da78b74d2c50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="52bad56f1cedf5a7e96bfe3d7dae91ef" ns2:_="">
     <xsd:import namespace="3f931156-b907-4802-85d4-da78b74d2c50"/>
@@ -14551,19 +14533,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="3f931156-b907-4802-85d4-da78b74d2c50">ZQWJEHJ6PPKV-702331974-10646</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="3f931156-b907-4802-85d4-da78b74d2c50">
-      <Url>https://sharepoint.corp.ovh.com/cdmo/_layouts/15/DocIdRedir.aspx?ID=ZQWJEHJ6PPKV-702331974-10646</Url>
-      <Description>ZQWJEHJ6PPKV-702331974-10646</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A7A2FDBE-E304-4784-B8F6-4B5BC2D4BFC5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -14571,15 +14549,17 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A46BBF6-FA99-4790-AC05-0112DDF87C39}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDAB445C-65E8-4095-B725-2E676BF1AE69}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14595,14 +14575,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36F60EC0-34C7-430C-980D-5238BA26FB73}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3f931156-b907-4802-85d4-da78b74d2c50"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>